<commit_message>
updated with shareable links
</commit_message>
<xml_diff>
--- a/Export2017URL.xlsx
+++ b/Export2017URL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="201">
   <si>
     <t>Metro</t>
   </si>
@@ -32,604 +32,601 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475977706</t>
-  </si>
-  <si>
     <t>Providence, RI</t>
   </si>
   <si>
     <t>Columbia, SC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475978663</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475949096</t>
-  </si>
-  <si>
     <t>Salt Lake City, UT</t>
   </si>
   <si>
     <t>Birmingham, AL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475950408</t>
-  </si>
-  <si>
     <t>Albany, NY</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475943638</t>
-  </si>
-  <si>
     <t>Orlando, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475941590</t>
-  </si>
-  <si>
     <t>Fresno, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475953052</t>
-  </si>
-  <si>
     <t>Omaha, NE-IA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475931184</t>
-  </si>
-  <si>
     <t>Jacksonville, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475888561</t>
-  </si>
-  <si>
     <t>Ogden, UT</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475944476</t>
-  </si>
-  <si>
     <t>Chicago, IL-IN-WI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475911556</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475925074</t>
-  </si>
-  <si>
     <t>North Port, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475901828</t>
-  </si>
-  <si>
     <t>Dayton, OH</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475907760</t>
-  </si>
-  <si>
     <t>Philadelphia, PA-NJ-DE</t>
   </si>
   <si>
     <t>Sacramento, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475902388</t>
-  </si>
-  <si>
     <t>St. Louis - MO-IL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475889527</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475907030</t>
-  </si>
-  <si>
     <t>New York, NY-NJ-PA</t>
   </si>
   <si>
     <t>Greenville, SC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475850479</t>
-  </si>
-  <si>
     <t>Bridgeport, CT</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475904468</t>
-  </si>
-  <si>
     <t>El Paso, TX</t>
   </si>
   <si>
-    <t>https://app.box.com/files/0/f/32639430129/1/f_199475859868</t>
-  </si>
-  <si>
     <t>Kansas City, MO-KS</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475860139</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475895153</t>
-  </si>
-  <si>
     <t>Springfield, MA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475887478</t>
-  </si>
-  <si>
     <t>Tucson, AZ</t>
   </si>
   <si>
     <t>Worcester, MA-CT</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475885940</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475851950</t>
-  </si>
-  <si>
     <t>Chattanooga, TN-GA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475846880</t>
-  </si>
-  <si>
     <t>San Jose, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475858308</t>
-  </si>
-  <si>
     <t>Oxnard, CA</t>
   </si>
   <si>
     <t>Rochester, NY</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475821428</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475832431</t>
-  </si>
-  <si>
     <t>Columbus, OH</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475844105</t>
-  </si>
-  <si>
     <t>Provo, UT</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475817764</t>
-  </si>
-  <si>
     <t>Cape Coral, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475809906</t>
-  </si>
-  <si>
     <t>Cleveland, OH</t>
   </si>
   <si>
     <t>Raleigh, NC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475771438</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475795243</t>
-  </si>
-  <si>
     <t>San Francisco, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475789612</t>
-  </si>
-  <si>
     <t>Youngstown, OH-PA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475809139</t>
-  </si>
-  <si>
     <t>Buffalo, NY</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475793315</t>
-  </si>
-  <si>
     <t>Boise City, ID</t>
   </si>
   <si>
     <t>Augusta, GA-SC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475764855</t>
-  </si>
-  <si>
     <t>Winston-Salem, NC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475773850</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/1/f/32639430129/1/f_199475799838</t>
-  </si>
-  <si>
     <t>Colorado Springs, CO</t>
   </si>
   <si>
     <t>Houston, TX</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475774179</t>
-  </si>
-  <si>
     <t>New Orleans, LA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475751659</t>
-  </si>
-  <si>
     <t>Scranton, PA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475744384</t>
-  </si>
-  <si>
     <t>Hartford, CT</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475734974</t>
-  </si>
-  <si>
     <t>Wichita, KS</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475753517</t>
-  </si>
-  <si>
     <t>Lakeland, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475763013</t>
-  </si>
-  <si>
     <t>Stockton, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475732903</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475760596</t>
-  </si>
-  <si>
     <t>Las Vegas, NV</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475753699</t>
-  </si>
-  <si>
     <t>Atlanta, GA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475745953</t>
-  </si>
-  <si>
     <t>Richmond, VA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475726368</t>
-  </si>
-  <si>
     <t>Toledo, OH</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475716561</t>
-  </si>
-  <si>
     <t>San Diego, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475742932</t>
-  </si>
-  <si>
     <t>Dallas, TX</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475743784</t>
-  </si>
-  <si>
     <t>Spokane, WA</t>
   </si>
   <si>
     <t>Allentown, PA-NJ</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475719771</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475724954</t>
-  </si>
-  <si>
     <t>New Haven, CT</t>
   </si>
   <si>
     <t>Baltimore, MD</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475731875</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475678500</t>
-  </si>
-  <si>
     <t>Boston, MA-NH</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475673672</t>
-  </si>
-  <si>
     <t>Urban Honolulu, HI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/2/f/32639430129/1/f_199475688298</t>
-  </si>
-  <si>
     <t>Denver</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475706276</t>
-  </si>
-  <si>
     <t>Tulsa, OK</t>
   </si>
   <si>
     <t>Palm Bay, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475685806</t>
-  </si>
-  <si>
     <t>Albuquerque, NM</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475691469</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475662402</t>
-  </si>
-  <si>
     <t>Bakersfield, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475671207</t>
-  </si>
-  <si>
     <t>Portland, OR-WA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475646367</t>
-  </si>
-  <si>
     <t>Los Angeles, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475659185</t>
-  </si>
-  <si>
     <t>Syracuse, NY</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475670262</t>
-  </si>
-  <si>
     <t>Louisville, KY-IN</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475642554</t>
-  </si>
-  <si>
     <t>Seattle, WA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475623344</t>
-  </si>
-  <si>
     <t>Little Rock, AR</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475648223</t>
-  </si>
-  <si>
     <t>Harrisburg, PA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475631263</t>
-  </si>
-  <si>
     <t>Oklahoma City, OK</t>
   </si>
   <si>
     <t>Jackson, MS</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475626431</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475620718</t>
-  </si>
-  <si>
     <t>Akron, OH</t>
   </si>
   <si>
     <t>Deltona, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475609764</t>
-  </si>
-  <si>
     <t>McAllen, TX</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475596303</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475591788</t>
-  </si>
-  <si>
     <t>Des Moines, IA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475616114</t>
-  </si>
-  <si>
     <t>Nashville, TN</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475615418</t>
-  </si>
-  <si>
     <t>Austin, TX</t>
   </si>
   <si>
     <t>San Antonio, TX</t>
   </si>
   <si>
-    <t>https://app.box.com/files/3/f/32639430129/1/f_199475624819</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475619650</t>
-  </si>
-  <si>
     <t>Milwaukee, WI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475615648</t>
-  </si>
-  <si>
     <t>Knoxville, TN</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475605462</t>
-  </si>
-  <si>
     <t>Cincinnati, OH-KY-IN</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475561227</t>
-  </si>
-  <si>
     <t>Madison, WI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475576229</t>
-  </si>
-  <si>
     <t>Washington, DC-VA-MD</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475596232</t>
-  </si>
-  <si>
     <t>Minneapolis, MN-WI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475561619</t>
-  </si>
-  <si>
     <t>Greensboro, NC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475565542</t>
-  </si>
-  <si>
     <t>Indianapolis, IN</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475598240</t>
-  </si>
-  <si>
     <t>Tampa, FL</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475566033</t>
-  </si>
-  <si>
     <t>Memphis, TN-MS-AR</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475589320</t>
-  </si>
-  <si>
     <t>Charleston, SC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475589084</t>
-  </si>
-  <si>
     <t>Miami, FL</t>
   </si>
   <si>
     <t>Baton Rouge, LA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475553386</t>
-  </si>
-  <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475538919</t>
-  </si>
-  <si>
     <t>Riverside, CA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475550119</t>
-  </si>
-  <si>
     <t>Charlotte, NC-SC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475562445</t>
-  </si>
-  <si>
     <t>Virginia Beach, VA-NC</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475545809</t>
-  </si>
-  <si>
     <t>Pittsburgh, PA</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475506201</t>
-  </si>
-  <si>
     <t>Detroit, MI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475475903</t>
-  </si>
-  <si>
     <t>Phoenix, AZ</t>
   </si>
   <si>
     <t>Grand Rapids, MI</t>
   </si>
   <si>
-    <t>https://app.box.com/files/4/f/32639430129/1/f_199475533418</t>
+    <t>https://app.box.com/s/d77uxmvezov4s9a2038r9wlk172x6a3p</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/5hy3kvdletjnq6m2ka0t5r5w9g5sy2tr</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/wgsiaqga28ikpyg5sgjopw5kpthv7838</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/yvzax0ux4yewqdu52bqkkywlrwmq2wc1</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/zhe7utx2b44azuy6t43xylduzba0imn6</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/6cvo5iabo46qief725kmhiso8lr0n7wm</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/zvkadp9rt3byf239wtvyi0x72g807qy6</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/mx46991d9tgasl84mwovmqy7ruoivkl2</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/4klh6lp51s7zkcbpl42v0bfabrqg26n4</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/kuxh2m7hivpl2cn8ulcvsz3o75rl9hui</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/447t1kf4m2c2ur45nsemexxvh53qnmua</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/9vja8t5vpspt3ricktvinne2sf1s2efb</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/539puh7d9g2vtr71hdn4mkxtuja7zipj</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/c2lniw9ft0hmqsqfzwaqgm8lxe528y6x</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/bdzugolu43uvqi28iy9l2zpy5bnywj07</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/amztltk6ghexgzpc1aklhxer5m3pv3gf</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/afrfgbyp61qvubu9hhbizkrgy15wz0l1</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/gg8d4l8ydp1hlp5evjlc3ni5wh4231rp</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/mewhfriuxza0dzjy89crsqst5rb2eg5y</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/csg6suwbv8rf8d0aos9sa9kuj3gmg35x</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/f6t61znoum14grdefcq6u2c8s6etphrt</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/3e1ccjd95b05c5g823rs9h2abyvgieyf</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/xi3r9292cdpwdtq7trj182xgxkljt3g9</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/b0gbyq8o8bxdbbzigbj3nwplq4ex51e4</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/2stq4ixcam7n5a2gj2gy8vafbhuaczdn</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/jmcdppmzabtz1m4zbb9iozqh2f80z1bl</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/0ogsbfdjbin16e14e7hitb9dgwwu6h6r</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/01z1crlc099ear5bnoignri6dhjnoypi</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/ro4o4x3jbt6yhg9yb90083znpagf4wav</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/vjrepbofxi6vffulvuxc1tjsn7uq7bl0</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/7k9ueijy6oci6fv3gz0lwo9xv2kq45wy</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/o2ehkxqaykybouqguskqbm4ernuc2egz</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/b6faqzsa063oyapv36650w50r2mk636l</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/tll6785bc9rkie7cvubmrvf9zdb46wnv</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/si65u9lgbgyw46yjk6zbto4udmcanzlr</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/u8rwbhwsq2cmj0hjewnfinrhu6x2bulz</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/6vx2yw4k12t9sg7lgn7a4ml4x3gz7as0</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/k76faxp7iz1ztsewbzn8g8zo860xtm3x</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/7sklwkpt47hvjkw18v2660xi20423jab</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/hv0opmxx4bky9mpc4i1vche1kikqy8fa</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/ydyweu3j5crqe52gw8ri4d2bvi5yet6h</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/dnbjf70f0pggrvwbnfgbi7m62yo2re3q</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/2k6xr1l14wglhkklayy0bbh246dgby1m</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/7rkk0mxg3tvqlvup5i200v1jgmt5p4ke</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/vwo6r6e4je0f5my616x4nfvo5loee59q</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/byj4jz22lkk87nq6a0qu91b1der77vnh</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/qrkt5ydl61buls544rwy74sqn7bvcxhd</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/vfahoja8tiuiv361rj243qq6tztfytnr</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/jc7i6k7qlk67uhbr0x0gmqbq803s4vnx</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/2x52j7spkbc2xt6n7b3z24qolnnwe8mi</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/7rpy2aim8bmnhvvsayi661kdy7bxysk9</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/yocr8haqu5i6joakssjj2ly4veo551v9</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/9sbg6x6rrradynmvc8gzizh7wwfc2eg6</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/8szcbmc1dkzfondgg3g6qw5s8nzflgej</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/g9my2scn89veejhkovpgtp9hmhh3t636</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/p750nl5h8x2tpdnclt68y56narnha876</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/svgfhnmfc79i7tnq3560q7v0h564vtt1</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/7altonwlb0taqu964ppd6j25ztxyb4hl</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/jngkfveg4cftlu6ufchraum9vfjg8lg9</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/2vzuvz58l4mn2dezvnefn5cwqpwbqkvb</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/aterzgk2o0qsa4wc7vafiiqk1zousk20</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/hwe047jcy5thnx9vlewhmhamrtup0s3i</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/lt1lcqau0j34l6ecs34s1v0y4rfkkva2</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/35xq0wcxjb3nfsc6wfaiwemrqis8vq3b</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/bhb0kbarjmkojr5npd4upvoq4vdmdtgs</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/wkkzv29iojk9isswrmd06gcgx52ys74v</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/upg9k8n4ik2hnftiiwix4z597lnpumr0</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/otq18o53pb0qybgq1186iqwww2d44c9v</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/yl5x0kt1c14wlyre3jsofnwmf7lggviv</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/nx6bwbz6kjn5wsvng7w5x146pa7uufyj</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/53u8r0c9l7yj1mq3dhebmedngoyjeuby</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/7h1w9df1o2giiddb14lsrg2b4d7t3tff</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/i3b0so02qw7khfwj9ijtzphgq94ex2i4</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/0p16d1go51ubgcm56o97obmyapz31bqx</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/x1myzf8lq1zu3jjeygb232vlgnq5w0a1</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/a4viesod7b4otjux5wfn2w4ensy1gn5n</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/hvbgougjji1q0yduqjuwdkgv5mc0o61i</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/9m39pi0hrzo9lv3ekc0cvgf0ti1csl5s</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/azkaqrqp86chpvx51l41j74ga9acvqmx</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/s31isuuenvd9saodfaaroovzh7pz3rf3</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/a7zff4sd133u0k1uh9dwr9e91nk1nlx2</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/h83kfyuf8wiyuewjjgl45kmp7dg6napk</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/v9wkq1g1yvuq38w8it3ovycwa8v95aei</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/qfusm6c255s6ojgtrrx1rjrkoqissuah</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/h2bl4inohcj3tgy2uysls6u0qz8t60qa</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/rm7py0aazjwlmcmkqtpwv4geth2drwhz</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/5qi5nqcuobbj6c3luovmwrsmx92cnu3z</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/lzgd8hvhc3ybrilhkschpqnjtddyq961</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/ut9e80j8xkbch4uipqajy2x3rtyzx0ya</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/vxq50avh0fogaikxndmn7t6a24k5um6c</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/o0oms83c3hobkaf3yl8dilm9taocuj8g</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/pfn09hgddkf2t7iaslkmczp76iwaart2</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/76bygdrcu1gk6e5th4kpwvsf73f0knyz</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/a7wxpp3rd603eyugzep4ppvejngrwuid</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/rkz8gbphsq4jr2tmuk1h48gwjzrlbcqr</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/6o5rkhok02x9afuw9dluid0pe1ph81a1</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/y21t63awawtyksrolo9mfx8b35v522zx</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/4qkmmf0h9jlpfeazqjennkys7q85u65a</t>
+  </si>
+  <si>
+    <t>https://app.box.com/s/j62xkmdbl5bi91ov0ncl7s51hzki2n3g</t>
   </si>
 </sst>
 </file>
@@ -987,7 +984,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1005,802 +1004,802 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>77</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>186</v>
+        <v>94</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>191</v>
+        <v>96</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>155</v>
+        <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>89</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>146</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>169</v>
+        <v>85</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>185</v>
+        <v>93</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>163</v>
+        <v>82</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>173</v>
+        <v>87</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>195</v>
+        <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>193</v>
+        <v>97</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>171</v>
+        <v>86</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1809,8 +1808,19 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="B21" r:id="rId1"/>
+    <hyperlink ref="B72" r:id="rId2"/>
+    <hyperlink ref="B25" r:id="rId3"/>
+    <hyperlink ref="B79" r:id="rId4"/>
+    <hyperlink ref="B12" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId6"/>
+    <hyperlink ref="B65" r:id="rId7"/>
+    <hyperlink ref="B34" r:id="rId8"/>
+    <hyperlink ref="B64" r:id="rId9"/>
+    <hyperlink ref="B43" r:id="rId10"/>
+    <hyperlink ref="B62" r:id="rId11"/>
+    <hyperlink ref="B61" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>